<commit_message>
Auto-committed on 2023/02/10 週五 11:43:28.26
</commit_message>
<xml_diff>
--- a/Program/Other/LM083_底稿_ICS放款資料.xlsx
+++ b/Program/Other/LM083_底稿_ICS放款資料.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6709D01-D3A9-49B7-A824-D024CF2E6516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F9B009-8346-4A49-9E75-37A40675A1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="1091231" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1091231'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1091231'!$C$1:$M$1</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>貸款類別</t>
     <phoneticPr fontId="20" type="noConversion"/>
@@ -63,6 +63,10 @@
   </si>
   <si>
     <t>到期日</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>區隔帳冊</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
@@ -719,12 +723,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="43" applyFont="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="22" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1133,13 +1137,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1155,10 +1159,11 @@
     <col min="9" max="9" width="38.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="12.77734375" style="8" customWidth="1"/>
-    <col min="13" max="16384" width="7.88671875" style="5"/>
+    <col min="13" max="13" width="11" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="7.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="9" t="s">
@@ -1191,8 +1196,11 @@
       <c r="L1" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1205,8 +1213,9 @@
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1219,9 +1228,10 @@
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -1238,12 +1248,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1361,15 +1368,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B9D2A1-BA89-45DC-AE93-3DA87EF407BA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB68B5EA-1F45-4733-885D-3D5EBF0272F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1391,10 +1402,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB68B5EA-1F45-4733-885D-3D5EBF0272F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56B9D2A1-BA89-45DC-AE93-3DA87EF407BA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>